<commit_message>
Rename Swim - Splits to Swim - Pool
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -6219,10 +6219,10 @@
     <t>UI_Activity_List_SwimLap</t>
   </si>
   <si>
-    <t>Swim - Laps</t>
-  </si>
-  <si>
-    <t>Simmning - Etapper</t>
+    <t>Swim - Pool</t>
+  </si>
+  <si>
+    <t>Simmning - Bassäng</t>
   </si>
   <si>
     <t>UI_Activity_List_SWOLF</t>

</xml_diff>

<commit_message>
Rename Swim trail to _Splits - Swim_
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -6360,13 +6360,13 @@
     <t>UI_Activity_List_SwimLap</t>
   </si>
   <si>
-    <t>Swim - Pool</t>
+    <t>Splits - Swim</t>
   </si>
   <si>
     <t>Natación - Piscina</t>
   </si>
   <si>
-    <t>Simmning - Bassäng</t>
+    <t>Etapper - Simmning</t>
   </si>
   <si>
     <t>UI_Activity_List_SWOLF</t>

</xml_diff>